<commit_message>
Day wise pages ongoing
</commit_message>
<xml_diff>
--- a/docs/TracingManagement.xlsx
+++ b/docs/TracingManagement.xlsx
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
1st & 2nd edition time modified in Pages
</commit_message>
<xml_diff>
--- a/docs/TracingManagement.xlsx
+++ b/docs/TracingManagement.xlsx
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>PageList</t>
   </si>
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1163,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>6</v>
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>34</v>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>35</v>
@@ -1230,6 +1230,9 @@
         <v>3</v>
       </c>
       <c r="F12" s="4"/>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Generate Tracing ongoing (insert data into Traing and TracingDetail done)
</commit_message>
<xml_diff>
--- a/docs/TracingManagement.xlsx
+++ b/docs/TracingManagement.xlsx
@@ -64,22 +64,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>All = 7 days in a week
-/
-Name of Day in a week like Friday</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="M14" authorId="0">
       <text>
         <r>
@@ -116,6 +100,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>All = 7 days in a week
+/
+Name of Day in a week like Friday</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t>Active / Inactive</t>
@@ -136,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="1">
+    <comment ref="E35" authorId="1">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>PageList</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>Employees</t>
+  </si>
+  <si>
+    <t>TracingTime_1st_edition</t>
+  </si>
+  <si>
+    <t>TracingTime_2nd_edition</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -492,7 +498,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1077,15 +1082,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31:U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
@@ -1141,10 +1146,10 @@
       <c r="J8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="22" t="s">
+      <c r="Q8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="22"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="3" t="s">
@@ -1242,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4"/>
       <c r="J13" s="1" t="s">
@@ -1253,8 +1258,8 @@
       <c r="B14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>36</v>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F14" s="18"/>
       <c r="J14" s="1" t="s">
@@ -1295,10 +1300,10 @@
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="E15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="19"/>
+      <c r="E15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="18"/>
       <c r="J15" s="12" t="s">
         <v>25</v>
       </c>
@@ -1315,6 +1320,9 @@
       <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:23">
+      <c r="E16" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1363,9 +1371,6 @@
       <c r="W18" s="1"/>
     </row>
     <row r="19" spans="4:23">
-      <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="J19" s="13" t="s">
         <v>29</v>
       </c>
@@ -1382,11 +1387,11 @@
       <c r="W19" s="1"/>
     </row>
     <row r="20" spans="4:23">
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>39</v>
+      <c r="E20" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J20" s="13" t="s">
         <v>30</v>
@@ -1405,7 +1410,7 @@
     </row>
     <row r="21" spans="4:23">
       <c r="E21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1420,6 +1425,9 @@
       <c r="W21" s="1"/>
     </row>
     <row r="22" spans="4:23">
+      <c r="E22" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1447,9 +1455,6 @@
     </row>
     <row r="24" spans="4:23">
       <c r="D24" s="17"/>
-      <c r="E24" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1466,8 +1471,8 @@
       <c r="D25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>41</v>
+      <c r="E25" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1486,7 +1491,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1501,6 +1506,9 @@
       <c r="W26" s="1"/>
     </row>
     <row r="27" spans="4:23">
+      <c r="E27" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1519,7 +1527,7 @@
       </c>
     </row>
     <row r="30" spans="4:23">
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="20" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1527,7 +1535,6 @@
       <c r="D31" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="4:23">
       <c r="D32" t="s">
@@ -1536,20 +1543,20 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="5:8">
+      <c r="E33" s="1"/>
       <c r="H33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="5:8">
-      <c r="E34" s="14" t="s">
-        <v>41</v>
-      </c>
       <c r="F34" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="5:8">
-      <c r="E35" s="1"/>
+      <c r="E35" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="H35" s="2" t="s">
         <v>0</v>
@@ -1571,6 +1578,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="5:8">
+      <c r="E39" s="1"/>
       <c r="H39" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>